<commit_message>
2.Add new tests and refactor code
</commit_message>
<xml_diff>
--- a/pr7_tretyakov_sergey (4) (2).xlsx
+++ b/pr7_tretyakov_sergey (4) (2).xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
@@ -652,7 +652,7 @@
         <sz val="11"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
-        <charset val="204"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Login must contain only alphanumeric characters and contain at least 6 characters</t>
     </r>
@@ -701,7 +701,7 @@
     <t xml:space="preserve">Checking the start page</t>
   </si>
   <si>
-    <t xml:space="preserve">Prerequisite: Open link "https://inventory.edu-netcracker.com/pages/startpage.xhtml"</t>
+    <t xml:space="preserve">Prerequisite: 1) Pre-registration in the system 2) Open link "https://inventory.edu-netcracker.com/pages/startpage.xhtml"</t>
   </si>
   <si>
     <t xml:space="preserve">TC_15.1</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">3.Get text of Input textbox</t>
   </si>
   <si>
-    <t xml:space="preserve">4.Get text of Software Logo link</t>
+    <t xml:space="preserve">4.Get text and link of Software Logo image-link</t>
   </si>
   <si>
     <t xml:space="preserve">5.Get text of Log out link</t>
@@ -929,7 +929,7 @@
     <t xml:space="preserve">TC_16.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Checking the "Post Terminal" object</t>
+    <t xml:space="preserve">Checking the "Post terminal" object</t>
   </si>
   <si>
     <t xml:space="preserve">6.Click on the "Rack" object</t>
@@ -971,7 +971,7 @@
     <t xml:space="preserve">TC_16.8</t>
   </si>
   <si>
-    <t xml:space="preserve">Checking the "Pay Box " object</t>
+    <t xml:space="preserve">Checking the "Pay Box" object</t>
   </si>
   <si>
     <t xml:space="preserve">7.Click on the "Pay Box (s)" button</t>
@@ -1177,6 +1177,9 @@
     <t xml:space="preserve">TC_17.7</t>
   </si>
   <si>
+    <t xml:space="preserve">Checking the "Post Terminal" object</t>
+  </si>
+  <si>
     <t xml:space="preserve">16.Get objects attribute text data</t>
   </si>
   <si>
@@ -1186,9 +1189,6 @@
     <t xml:space="preserve">TC_17.8</t>
   </si>
   <si>
-    <t xml:space="preserve">Checking the "Pay Box" object</t>
-  </si>
-  <si>
     <t xml:space="preserve">15.Get objects attribute text data</t>
   </si>
   <si>
@@ -1330,7 +1330,7 @@
     <t xml:space="preserve">User16</t>
   </si>
   <si>
-    <t xml:space="preserve">Name - "Russhia"; Continent - Eurasia; Language - "Russhian"</t>
+    <t xml:space="preserve">Name — random name; Continent - Eurasia; Language — random language</t>
   </si>
   <si>
     <t xml:space="preserve">User17</t>
@@ -1690,7 +1690,7 @@
       <sz val="11"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1745,8 +1745,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF454FA1"/>
-        <bgColor rgb="FF666699"/>
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -1840,7 +1840,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="85">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1981,54 +1981,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2217,7 +2173,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2274,7 +2234,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -2286,7 +2246,7 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF454FA1"/>
+      <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -2300,8 +2260,8 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E455" activeCellId="0" sqref="E455"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A247" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B258" activeCellId="0" sqref="B258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3740,7 +3700,7 @@
       </c>
       <c r="D159" s="3"/>
     </row>
-    <row r="160" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="7"/>
       <c r="B160" s="3"/>
       <c r="C160" s="25" t="s">
@@ -5155,1106 +5115,1106 @@
       <c r="D323" s="27"/>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A324" s="35" t="s">
+      <c r="A324" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="B324" s="36" t="s">
+      <c r="B324" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C324" s="37" t="s">
+      <c r="C324" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D324" s="38" t="s">
+      <c r="D324" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="35"/>
-      <c r="B325" s="36"/>
-      <c r="C325" s="37" t="s">
+      <c r="A325" s="7"/>
+      <c r="B325" s="8"/>
+      <c r="C325" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="D325" s="38"/>
+      <c r="D325" s="3"/>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="35"/>
-      <c r="B326" s="36"/>
-      <c r="C326" s="39" t="s">
+      <c r="A326" s="7"/>
+      <c r="B326" s="8"/>
+      <c r="C326" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="D326" s="38"/>
+      <c r="D326" s="3"/>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A327" s="35"/>
-      <c r="B327" s="36"/>
-      <c r="C327" s="40" t="s">
+      <c r="A327" s="7"/>
+      <c r="B327" s="8"/>
+      <c r="C327" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="D327" s="38"/>
+      <c r="D327" s="3"/>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="35"/>
-      <c r="B328" s="36"/>
-      <c r="C328" s="40" t="s">
+      <c r="A328" s="7"/>
+      <c r="B328" s="8"/>
+      <c r="C328" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="D328" s="38"/>
+      <c r="D328" s="3"/>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="35"/>
-      <c r="B329" s="36"/>
-      <c r="C329" s="41" t="s">
+      <c r="A329" s="7"/>
+      <c r="B329" s="8"/>
+      <c r="C329" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="D329" s="38"/>
+      <c r="D329" s="3"/>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="35"/>
-      <c r="B330" s="36"/>
-      <c r="C330" s="37" t="s">
+      <c r="A330" s="7"/>
+      <c r="B330" s="8"/>
+      <c r="C330" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="D330" s="38"/>
+      <c r="D330" s="3"/>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A331" s="35"/>
-      <c r="B331" s="36"/>
-      <c r="C331" s="37" t="s">
+      <c r="A331" s="7"/>
+      <c r="B331" s="8"/>
+      <c r="C331" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="D331" s="38"/>
+      <c r="D331" s="3"/>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="42"/>
-      <c r="B332" s="43" t="s">
+      <c r="A332" s="29"/>
+      <c r="B332" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C332" s="43"/>
-      <c r="D332" s="43"/>
+      <c r="C332" s="27"/>
+      <c r="D332" s="27"/>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A333" s="35" t="s">
+      <c r="A333" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="B333" s="36" t="s">
+      <c r="B333" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C333" s="37" t="s">
+      <c r="C333" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D333" s="38" t="s">
+      <c r="D333" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="35"/>
-      <c r="B334" s="36"/>
-      <c r="C334" s="39" t="s">
+      <c r="A334" s="7"/>
+      <c r="B334" s="8"/>
+      <c r="C334" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D334" s="38"/>
+      <c r="D334" s="3"/>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="35"/>
-      <c r="B335" s="36"/>
-      <c r="C335" s="37" t="s">
+      <c r="A335" s="7"/>
+      <c r="B335" s="8"/>
+      <c r="C335" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="D335" s="38"/>
+      <c r="D335" s="3"/>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A336" s="35"/>
-      <c r="B336" s="36"/>
-      <c r="C336" s="37" t="s">
+      <c r="A336" s="7"/>
+      <c r="B336" s="8"/>
+      <c r="C336" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D336" s="38"/>
+      <c r="D336" s="3"/>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="35"/>
-      <c r="B337" s="36"/>
-      <c r="C337" s="37" t="s">
+      <c r="A337" s="7"/>
+      <c r="B337" s="8"/>
+      <c r="C337" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="D337" s="38"/>
+      <c r="D337" s="3"/>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="35"/>
-      <c r="B338" s="36"/>
-      <c r="C338" s="37" t="s">
+      <c r="A338" s="7"/>
+      <c r="B338" s="8"/>
+      <c r="C338" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="D338" s="38"/>
+      <c r="D338" s="3"/>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="35"/>
-      <c r="B339" s="36"/>
-      <c r="C339" s="37" t="s">
+      <c r="A339" s="7"/>
+      <c r="B339" s="8"/>
+      <c r="C339" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="D339" s="38"/>
+      <c r="D339" s="3"/>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A340" s="35"/>
-      <c r="B340" s="36"/>
-      <c r="C340" s="37" t="s">
+      <c r="A340" s="7"/>
+      <c r="B340" s="8"/>
+      <c r="C340" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="D340" s="38"/>
+      <c r="D340" s="3"/>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="35"/>
-      <c r="B341" s="36"/>
-      <c r="C341" s="37" t="s">
+      <c r="A341" s="7"/>
+      <c r="B341" s="8"/>
+      <c r="C341" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="D341" s="38"/>
+      <c r="D341" s="3"/>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="35"/>
-      <c r="B342" s="36"/>
-      <c r="C342" s="37" t="s">
+      <c r="A342" s="7"/>
+      <c r="B342" s="8"/>
+      <c r="C342" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="D342" s="38"/>
+      <c r="D342" s="3"/>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A343" s="35"/>
-      <c r="B343" s="36"/>
-      <c r="C343" s="37" t="s">
+      <c r="A343" s="7"/>
+      <c r="B343" s="8"/>
+      <c r="C343" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="D343" s="38"/>
+      <c r="D343" s="3"/>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A344" s="42"/>
-      <c r="B344" s="43" t="s">
+      <c r="A344" s="29"/>
+      <c r="B344" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C344" s="43"/>
-      <c r="D344" s="43"/>
+      <c r="C344" s="27"/>
+      <c r="D344" s="27"/>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A345" s="35" t="s">
+      <c r="A345" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="B345" s="36" t="s">
+      <c r="B345" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="C345" s="37" t="s">
+      <c r="C345" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D345" s="44" t="s">
+      <c r="D345" s="35" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="35"/>
-      <c r="B346" s="36"/>
-      <c r="C346" s="39" t="s">
+      <c r="A346" s="7"/>
+      <c r="B346" s="8"/>
+      <c r="C346" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D346" s="44"/>
+      <c r="D346" s="35"/>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="35"/>
-      <c r="B347" s="36"/>
-      <c r="C347" s="37" t="s">
+      <c r="A347" s="7"/>
+      <c r="B347" s="8"/>
+      <c r="C347" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D347" s="44"/>
+      <c r="D347" s="35"/>
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A348" s="35"/>
-      <c r="B348" s="36"/>
-      <c r="C348" s="37" t="s">
+      <c r="A348" s="7"/>
+      <c r="B348" s="8"/>
+      <c r="C348" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="D348" s="44"/>
+      <c r="D348" s="35"/>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="35"/>
-      <c r="B349" s="36"/>
-      <c r="C349" s="37" t="s">
+      <c r="A349" s="7"/>
+      <c r="B349" s="8"/>
+      <c r="C349" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="D349" s="44"/>
+      <c r="D349" s="35"/>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A350" s="35"/>
-      <c r="B350" s="36"/>
-      <c r="C350" s="37" t="s">
+      <c r="A350" s="7"/>
+      <c r="B350" s="8"/>
+      <c r="C350" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="D350" s="44"/>
+      <c r="D350" s="35"/>
     </row>
     <row r="351" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A351" s="35"/>
-      <c r="B351" s="36"/>
-      <c r="C351" s="37" t="s">
+      <c r="A351" s="7"/>
+      <c r="B351" s="8"/>
+      <c r="C351" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="D351" s="44"/>
+      <c r="D351" s="35"/>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="35"/>
-      <c r="B352" s="36"/>
-      <c r="C352" s="45" t="s">
+      <c r="A352" s="7"/>
+      <c r="B352" s="8"/>
+      <c r="C352" s="33" t="s">
         <v>329</v>
       </c>
-      <c r="D352" s="44"/>
+      <c r="D352" s="35"/>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="35"/>
-      <c r="B353" s="36"/>
-      <c r="C353" s="45" t="s">
+      <c r="A353" s="7"/>
+      <c r="B353" s="8"/>
+      <c r="C353" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="D353" s="44"/>
+      <c r="D353" s="35"/>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="42"/>
-      <c r="B354" s="43" t="s">
+      <c r="A354" s="29"/>
+      <c r="B354" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C354" s="43"/>
-      <c r="D354" s="43"/>
+      <c r="C354" s="27"/>
+      <c r="D354" s="27"/>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A355" s="35" t="s">
+      <c r="A355" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="B355" s="36" t="s">
+      <c r="B355" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="C355" s="37" t="s">
+      <c r="C355" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D355" s="38" t="s">
+      <c r="D355" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="35"/>
-      <c r="B356" s="36"/>
-      <c r="C356" s="39" t="s">
+      <c r="A356" s="7"/>
+      <c r="B356" s="8"/>
+      <c r="C356" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D356" s="38"/>
+      <c r="D356" s="3"/>
     </row>
     <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="35"/>
-      <c r="B357" s="36"/>
-      <c r="C357" s="37" t="s">
+      <c r="A357" s="7"/>
+      <c r="B357" s="8"/>
+      <c r="C357" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D357" s="38"/>
+      <c r="D357" s="3"/>
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="35"/>
-      <c r="B358" s="36"/>
-      <c r="C358" s="39" t="s">
+      <c r="A358" s="7"/>
+      <c r="B358" s="8"/>
+      <c r="C358" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="D358" s="38"/>
+      <c r="D358" s="3"/>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="35"/>
-      <c r="B359" s="36"/>
-      <c r="C359" s="39" t="s">
+      <c r="A359" s="7"/>
+      <c r="B359" s="8"/>
+      <c r="C359" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="D359" s="38"/>
+      <c r="D359" s="3"/>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="35"/>
-      <c r="B360" s="36"/>
-      <c r="C360" s="39" t="s">
+      <c r="A360" s="7"/>
+      <c r="B360" s="8"/>
+      <c r="C360" s="25" t="s">
         <v>247</v>
       </c>
-      <c r="D360" s="38"/>
+      <c r="D360" s="3"/>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A361" s="35"/>
-      <c r="B361" s="36"/>
-      <c r="C361" s="39" t="s">
+      <c r="A361" s="7"/>
+      <c r="B361" s="8"/>
+      <c r="C361" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="D361" s="38"/>
+      <c r="D361" s="3"/>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="35"/>
-      <c r="B362" s="36"/>
-      <c r="C362" s="39" t="s">
+      <c r="A362" s="7"/>
+      <c r="B362" s="8"/>
+      <c r="C362" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="D362" s="38"/>
+      <c r="D362" s="3"/>
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A363" s="35"/>
-      <c r="B363" s="36"/>
-      <c r="C363" s="39" t="s">
+      <c r="A363" s="7"/>
+      <c r="B363" s="8"/>
+      <c r="C363" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="D363" s="38"/>
+      <c r="D363" s="3"/>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A364" s="35"/>
-      <c r="B364" s="36"/>
-      <c r="C364" s="39" t="s">
+      <c r="A364" s="7"/>
+      <c r="B364" s="8"/>
+      <c r="C364" s="25" t="s">
         <v>333</v>
       </c>
-      <c r="D364" s="38"/>
+      <c r="D364" s="3"/>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A365" s="46"/>
-      <c r="B365" s="43" t="s">
+      <c r="A365" s="9"/>
+      <c r="B365" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C365" s="43"/>
-      <c r="D365" s="43"/>
+      <c r="C365" s="27"/>
+      <c r="D365" s="27"/>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A366" s="35" t="s">
+      <c r="A366" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="B366" s="36" t="s">
+      <c r="B366" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="C366" s="37" t="s">
+      <c r="C366" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D366" s="38" t="s">
+      <c r="D366" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A367" s="35"/>
-      <c r="B367" s="36"/>
-      <c r="C367" s="39" t="s">
+      <c r="A367" s="7"/>
+      <c r="B367" s="8"/>
+      <c r="C367" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D367" s="38"/>
+      <c r="D367" s="3"/>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A368" s="35"/>
-      <c r="B368" s="36"/>
-      <c r="C368" s="37" t="s">
+      <c r="A368" s="7"/>
+      <c r="B368" s="8"/>
+      <c r="C368" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D368" s="38"/>
+      <c r="D368" s="3"/>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A369" s="35"/>
-      <c r="B369" s="36"/>
-      <c r="C369" s="39" t="s">
+      <c r="A369" s="7"/>
+      <c r="B369" s="8"/>
+      <c r="C369" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="D369" s="38"/>
+      <c r="D369" s="3"/>
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A370" s="35"/>
-      <c r="B370" s="36"/>
-      <c r="C370" s="37" t="s">
+      <c r="A370" s="7"/>
+      <c r="B370" s="8"/>
+      <c r="C370" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D370" s="38"/>
+      <c r="D370" s="3"/>
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A371" s="35"/>
-      <c r="B371" s="36"/>
-      <c r="C371" s="37" t="s">
+      <c r="A371" s="7"/>
+      <c r="B371" s="8"/>
+      <c r="C371" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="D371" s="38"/>
+      <c r="D371" s="3"/>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A372" s="35"/>
-      <c r="B372" s="36"/>
-      <c r="C372" s="37" t="s">
+      <c r="A372" s="7"/>
+      <c r="B372" s="8"/>
+      <c r="C372" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="D372" s="38"/>
+      <c r="D372" s="3"/>
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="35"/>
-      <c r="B373" s="36"/>
-      <c r="C373" s="37" t="s">
+      <c r="A373" s="7"/>
+      <c r="B373" s="8"/>
+      <c r="C373" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="D373" s="38"/>
+      <c r="D373" s="3"/>
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="35"/>
-      <c r="B374" s="36"/>
-      <c r="C374" s="37" t="s">
+      <c r="A374" s="7"/>
+      <c r="B374" s="8"/>
+      <c r="C374" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="D374" s="38"/>
+      <c r="D374" s="3"/>
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A375" s="35"/>
-      <c r="B375" s="36"/>
-      <c r="C375" s="39" t="s">
+      <c r="A375" s="7"/>
+      <c r="B375" s="8"/>
+      <c r="C375" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="D375" s="38"/>
+      <c r="D375" s="3"/>
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A376" s="35"/>
-      <c r="B376" s="36"/>
-      <c r="C376" s="39" t="s">
+      <c r="A376" s="7"/>
+      <c r="B376" s="8"/>
+      <c r="C376" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="D376" s="38"/>
+      <c r="D376" s="3"/>
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A377" s="35"/>
-      <c r="B377" s="36"/>
-      <c r="C377" s="39" t="s">
+      <c r="A377" s="7"/>
+      <c r="B377" s="8"/>
+      <c r="C377" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="D377" s="38"/>
+      <c r="D377" s="3"/>
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A378" s="35"/>
-      <c r="B378" s="36"/>
-      <c r="C378" s="39" t="s">
+      <c r="A378" s="7"/>
+      <c r="B378" s="8"/>
+      <c r="C378" s="25" t="s">
         <v>335</v>
       </c>
-      <c r="D378" s="38"/>
+      <c r="D378" s="3"/>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A379" s="35"/>
-      <c r="B379" s="36"/>
-      <c r="C379" s="39" t="s">
+      <c r="A379" s="7"/>
+      <c r="B379" s="8"/>
+      <c r="C379" s="25" t="s">
         <v>336</v>
       </c>
-      <c r="D379" s="38"/>
+      <c r="D379" s="3"/>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A380" s="46"/>
-      <c r="B380" s="43" t="s">
+      <c r="A380" s="9"/>
+      <c r="B380" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C380" s="43"/>
-      <c r="D380" s="43"/>
+      <c r="C380" s="27"/>
+      <c r="D380" s="27"/>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A381" s="35" t="s">
+      <c r="A381" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="B381" s="36" t="s">
-        <v>265</v>
-      </c>
-      <c r="C381" s="37" t="s">
+      <c r="B381" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C381" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D381" s="38" t="s">
+      <c r="D381" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A382" s="35"/>
-      <c r="B382" s="36"/>
-      <c r="C382" s="39" t="s">
+      <c r="A382" s="7"/>
+      <c r="B382" s="8"/>
+      <c r="C382" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D382" s="38"/>
+      <c r="D382" s="3"/>
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="35"/>
-      <c r="B383" s="36"/>
-      <c r="C383" s="37" t="s">
+      <c r="A383" s="7"/>
+      <c r="B383" s="8"/>
+      <c r="C383" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D383" s="38"/>
+      <c r="D383" s="3"/>
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="35"/>
-      <c r="B384" s="36"/>
-      <c r="C384" s="39" t="s">
+      <c r="A384" s="7"/>
+      <c r="B384" s="8"/>
+      <c r="C384" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="D384" s="38"/>
+      <c r="D384" s="3"/>
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A385" s="35"/>
-      <c r="B385" s="36"/>
-      <c r="C385" s="37" t="s">
+      <c r="A385" s="7"/>
+      <c r="B385" s="8"/>
+      <c r="C385" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D385" s="38"/>
+      <c r="D385" s="3"/>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A386" s="35"/>
-      <c r="B386" s="36"/>
-      <c r="C386" s="37" t="s">
+      <c r="A386" s="7"/>
+      <c r="B386" s="8"/>
+      <c r="C386" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="D386" s="38"/>
+      <c r="D386" s="3"/>
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="35"/>
-      <c r="B387" s="36"/>
-      <c r="C387" s="37" t="s">
+      <c r="A387" s="7"/>
+      <c r="B387" s="8"/>
+      <c r="C387" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D387" s="38"/>
+      <c r="D387" s="3"/>
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="35"/>
-      <c r="B388" s="36"/>
-      <c r="C388" s="37" t="s">
+      <c r="A388" s="7"/>
+      <c r="B388" s="8"/>
+      <c r="C388" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="D388" s="38"/>
+      <c r="D388" s="3"/>
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="35"/>
-      <c r="B389" s="36"/>
-      <c r="C389" s="37" t="s">
+      <c r="A389" s="7"/>
+      <c r="B389" s="8"/>
+      <c r="C389" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="D389" s="38"/>
+      <c r="D389" s="3"/>
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A390" s="35"/>
-      <c r="B390" s="36"/>
-      <c r="C390" s="37" t="s">
+      <c r="A390" s="7"/>
+      <c r="B390" s="8"/>
+      <c r="C390" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="D390" s="38"/>
+      <c r="D390" s="3"/>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="35"/>
-      <c r="B391" s="36"/>
-      <c r="C391" s="37" t="s">
+      <c r="A391" s="7"/>
+      <c r="B391" s="8"/>
+      <c r="C391" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="D391" s="38"/>
+      <c r="D391" s="3"/>
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="35"/>
-      <c r="B392" s="36"/>
-      <c r="C392" s="39" t="s">
+      <c r="A392" s="7"/>
+      <c r="B392" s="8"/>
+      <c r="C392" s="25" t="s">
         <v>272</v>
       </c>
-      <c r="D392" s="38"/>
+      <c r="D392" s="3"/>
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A393" s="35"/>
-      <c r="B393" s="36"/>
-      <c r="C393" s="37" t="s">
+      <c r="A393" s="7"/>
+      <c r="B393" s="8"/>
+      <c r="C393" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="D393" s="38"/>
+      <c r="D393" s="3"/>
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A394" s="35"/>
-      <c r="B394" s="36"/>
-      <c r="C394" s="37" t="s">
+      <c r="A394" s="7"/>
+      <c r="B394" s="8"/>
+      <c r="C394" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="D394" s="38"/>
+      <c r="D394" s="3"/>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A395" s="35"/>
-      <c r="B395" s="36"/>
-      <c r="C395" s="37" t="s">
+      <c r="A395" s="7"/>
+      <c r="B395" s="8"/>
+      <c r="C395" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="D395" s="38"/>
+      <c r="D395" s="3"/>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="35"/>
-      <c r="B396" s="36"/>
-      <c r="C396" s="37" t="s">
-        <v>338</v>
-      </c>
-      <c r="D396" s="38"/>
+      <c r="A396" s="7"/>
+      <c r="B396" s="8"/>
+      <c r="C396" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D396" s="3"/>
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="35"/>
-      <c r="B397" s="36"/>
-      <c r="C397" s="37" t="s">
-        <v>339</v>
-      </c>
-      <c r="D397" s="38"/>
+      <c r="A397" s="7"/>
+      <c r="B397" s="8"/>
+      <c r="C397" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D397" s="3"/>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A398" s="46"/>
-      <c r="B398" s="43" t="s">
+      <c r="A398" s="9"/>
+      <c r="B398" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C398" s="43"/>
-      <c r="D398" s="43"/>
+      <c r="C398" s="27"/>
+      <c r="D398" s="27"/>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A399" s="35" t="s">
-        <v>340</v>
-      </c>
-      <c r="B399" s="36" t="s">
+      <c r="A399" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="C399" s="37" t="s">
+      <c r="B399" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C399" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D399" s="47" t="s">
+      <c r="D399" s="36" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="35"/>
-      <c r="B400" s="36"/>
-      <c r="C400" s="39" t="s">
+      <c r="A400" s="7"/>
+      <c r="B400" s="8"/>
+      <c r="C400" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D400" s="47"/>
+      <c r="D400" s="36"/>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="35"/>
-      <c r="B401" s="36"/>
-      <c r="C401" s="37" t="s">
+      <c r="A401" s="7"/>
+      <c r="B401" s="8"/>
+      <c r="C401" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D401" s="47"/>
+      <c r="D401" s="36"/>
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="35"/>
-      <c r="B402" s="36"/>
-      <c r="C402" s="39" t="s">
+      <c r="A402" s="7"/>
+      <c r="B402" s="8"/>
+      <c r="C402" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="D402" s="47"/>
+      <c r="D402" s="36"/>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="35"/>
-      <c r="B403" s="36"/>
-      <c r="C403" s="37" t="s">
+      <c r="A403" s="7"/>
+      <c r="B403" s="8"/>
+      <c r="C403" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D403" s="47"/>
+      <c r="D403" s="36"/>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="35"/>
-      <c r="B404" s="36"/>
-      <c r="C404" s="37" t="s">
+      <c r="A404" s="7"/>
+      <c r="B404" s="8"/>
+      <c r="C404" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="D404" s="47"/>
+      <c r="D404" s="36"/>
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="35"/>
-      <c r="B405" s="36"/>
-      <c r="C405" s="37" t="s">
+      <c r="A405" s="7"/>
+      <c r="B405" s="8"/>
+      <c r="C405" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="D405" s="47"/>
+      <c r="D405" s="36"/>
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="35"/>
-      <c r="B406" s="36"/>
-      <c r="C406" s="37" t="s">
+      <c r="A406" s="7"/>
+      <c r="B406" s="8"/>
+      <c r="C406" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="D406" s="47"/>
+      <c r="D406" s="36"/>
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A407" s="35"/>
-      <c r="B407" s="36"/>
-      <c r="C407" s="37" t="s">
+      <c r="A407" s="7"/>
+      <c r="B407" s="8"/>
+      <c r="C407" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="D407" s="47"/>
+      <c r="D407" s="36"/>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A408" s="35"/>
-      <c r="B408" s="36"/>
-      <c r="C408" s="37" t="s">
+      <c r="A408" s="7"/>
+      <c r="B408" s="8"/>
+      <c r="C408" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="D408" s="47"/>
+      <c r="D408" s="36"/>
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="35"/>
-      <c r="B409" s="36"/>
-      <c r="C409" s="37" t="s">
+      <c r="A409" s="7"/>
+      <c r="B409" s="8"/>
+      <c r="C409" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="D409" s="47"/>
+      <c r="D409" s="36"/>
     </row>
     <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="35"/>
-      <c r="B410" s="36"/>
-      <c r="C410" s="37" t="s">
+      <c r="A410" s="7"/>
+      <c r="B410" s="8"/>
+      <c r="C410" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="D410" s="47"/>
+      <c r="D410" s="36"/>
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="35"/>
-      <c r="B411" s="36"/>
-      <c r="C411" s="37" t="s">
+      <c r="A411" s="7"/>
+      <c r="B411" s="8"/>
+      <c r="C411" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D411" s="47"/>
+      <c r="D411" s="36"/>
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A412" s="35"/>
-      <c r="B412" s="36"/>
-      <c r="C412" s="37" t="s">
+      <c r="A412" s="7"/>
+      <c r="B412" s="8"/>
+      <c r="C412" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="D412" s="47"/>
+      <c r="D412" s="36"/>
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="35"/>
-      <c r="B413" s="36"/>
-      <c r="C413" s="37" t="s">
+      <c r="A413" s="7"/>
+      <c r="B413" s="8"/>
+      <c r="C413" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="D413" s="47"/>
+      <c r="D413" s="36"/>
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A414" s="35"/>
-      <c r="B414" s="36"/>
-      <c r="C414" s="37" t="s">
+      <c r="A414" s="7"/>
+      <c r="B414" s="8"/>
+      <c r="C414" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="D414" s="47"/>
+      <c r="D414" s="36"/>
     </row>
     <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="46"/>
-      <c r="B415" s="43" t="s">
+      <c r="A415" s="9"/>
+      <c r="B415" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C415" s="43"/>
-      <c r="D415" s="43"/>
+      <c r="C415" s="27"/>
+      <c r="D415" s="27"/>
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A416" s="35" t="s">
+      <c r="A416" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="B416" s="36" t="s">
+      <c r="B416" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="C416" s="37" t="s">
+      <c r="C416" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D416" s="47" t="s">
+      <c r="D416" s="36" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A417" s="35"/>
-      <c r="B417" s="36"/>
-      <c r="C417" s="39" t="s">
+      <c r="A417" s="7"/>
+      <c r="B417" s="8"/>
+      <c r="C417" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D417" s="47"/>
+      <c r="D417" s="36"/>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="35"/>
-      <c r="B418" s="36"/>
-      <c r="C418" s="37" t="s">
+      <c r="A418" s="7"/>
+      <c r="B418" s="8"/>
+      <c r="C418" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D418" s="47"/>
+      <c r="D418" s="36"/>
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A419" s="35"/>
-      <c r="B419" s="36"/>
-      <c r="C419" s="39" t="s">
+      <c r="A419" s="7"/>
+      <c r="B419" s="8"/>
+      <c r="C419" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="D419" s="47"/>
+      <c r="D419" s="36"/>
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="35"/>
-      <c r="B420" s="36"/>
-      <c r="C420" s="37" t="s">
+      <c r="A420" s="7"/>
+      <c r="B420" s="8"/>
+      <c r="C420" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D420" s="47"/>
+      <c r="D420" s="36"/>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="35"/>
-      <c r="B421" s="36"/>
-      <c r="C421" s="37" t="s">
+      <c r="A421" s="7"/>
+      <c r="B421" s="8"/>
+      <c r="C421" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="D421" s="47"/>
+      <c r="D421" s="36"/>
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="35"/>
-      <c r="B422" s="36"/>
-      <c r="C422" s="37" t="s">
+      <c r="A422" s="7"/>
+      <c r="B422" s="8"/>
+      <c r="C422" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="D422" s="47"/>
+      <c r="D422" s="36"/>
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="35"/>
-      <c r="B423" s="36"/>
-      <c r="C423" s="37" t="s">
+      <c r="A423" s="7"/>
+      <c r="B423" s="8"/>
+      <c r="C423" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="D423" s="47"/>
+      <c r="D423" s="36"/>
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="35"/>
-      <c r="B424" s="36"/>
-      <c r="C424" s="37" t="s">
+      <c r="A424" s="7"/>
+      <c r="B424" s="8"/>
+      <c r="C424" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="D424" s="47"/>
+      <c r="D424" s="36"/>
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="35"/>
-      <c r="B425" s="36"/>
-      <c r="C425" s="37" t="s">
+      <c r="A425" s="7"/>
+      <c r="B425" s="8"/>
+      <c r="C425" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="D425" s="47"/>
+      <c r="D425" s="36"/>
     </row>
     <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A426" s="35"/>
-      <c r="B426" s="36"/>
-      <c r="C426" s="37" t="s">
+      <c r="A426" s="7"/>
+      <c r="B426" s="8"/>
+      <c r="C426" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="D426" s="47"/>
+      <c r="D426" s="36"/>
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A427" s="35"/>
-      <c r="B427" s="36"/>
-      <c r="C427" s="37" t="s">
+      <c r="A427" s="7"/>
+      <c r="B427" s="8"/>
+      <c r="C427" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="D427" s="47"/>
+      <c r="D427" s="36"/>
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A428" s="35"/>
-      <c r="B428" s="36"/>
-      <c r="C428" s="37" t="s">
+      <c r="A428" s="7"/>
+      <c r="B428" s="8"/>
+      <c r="C428" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="D428" s="47"/>
+      <c r="D428" s="36"/>
     </row>
     <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="35"/>
-      <c r="B429" s="36"/>
-      <c r="C429" s="37" t="s">
+      <c r="A429" s="7"/>
+      <c r="B429" s="8"/>
+      <c r="C429" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="D429" s="47"/>
+      <c r="D429" s="36"/>
     </row>
     <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A430" s="35"/>
-      <c r="B430" s="36"/>
-      <c r="C430" s="37" t="s">
+      <c r="A430" s="7"/>
+      <c r="B430" s="8"/>
+      <c r="C430" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="D430" s="47"/>
+      <c r="D430" s="36"/>
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="35"/>
-      <c r="B431" s="36"/>
-      <c r="C431" s="37" t="s">
+      <c r="A431" s="7"/>
+      <c r="B431" s="8"/>
+      <c r="C431" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="D431" s="47"/>
+      <c r="D431" s="36"/>
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="46"/>
-      <c r="B432" s="43" t="s">
+      <c r="A432" s="9"/>
+      <c r="B432" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C432" s="43"/>
-      <c r="D432" s="43"/>
+      <c r="C432" s="27"/>
+      <c r="D432" s="27"/>
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A433" s="35" t="s">
+      <c r="A433" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="B433" s="36" t="s">
+      <c r="B433" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="C433" s="37" t="s">
+      <c r="C433" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D433" s="38" t="s">
+      <c r="D433" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="35"/>
-      <c r="B434" s="36"/>
-      <c r="C434" s="39" t="s">
+      <c r="A434" s="7"/>
+      <c r="B434" s="8"/>
+      <c r="C434" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="D434" s="38"/>
+      <c r="D434" s="3"/>
     </row>
     <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="35"/>
-      <c r="B435" s="36"/>
-      <c r="C435" s="37" t="s">
+      <c r="A435" s="7"/>
+      <c r="B435" s="8"/>
+      <c r="C435" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D435" s="38"/>
+      <c r="D435" s="3"/>
     </row>
     <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="35"/>
-      <c r="B436" s="36"/>
-      <c r="C436" s="39" t="s">
+      <c r="A436" s="7"/>
+      <c r="B436" s="8"/>
+      <c r="C436" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="D436" s="38"/>
+      <c r="D436" s="3"/>
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="35"/>
-      <c r="B437" s="36"/>
-      <c r="C437" s="37" t="s">
+      <c r="A437" s="7"/>
+      <c r="B437" s="8"/>
+      <c r="C437" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D437" s="38"/>
+      <c r="D437" s="3"/>
     </row>
     <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="35"/>
-      <c r="B438" s="36"/>
-      <c r="C438" s="37" t="s">
+      <c r="A438" s="7"/>
+      <c r="B438" s="8"/>
+      <c r="C438" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="D438" s="38"/>
+      <c r="D438" s="3"/>
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="35"/>
-      <c r="B439" s="36"/>
-      <c r="C439" s="37" t="s">
+      <c r="A439" s="7"/>
+      <c r="B439" s="8"/>
+      <c r="C439" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="D439" s="38"/>
+      <c r="D439" s="3"/>
     </row>
     <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="35"/>
-      <c r="B440" s="36"/>
-      <c r="C440" s="37" t="s">
+      <c r="A440" s="7"/>
+      <c r="B440" s="8"/>
+      <c r="C440" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="D440" s="38"/>
+      <c r="D440" s="3"/>
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="35"/>
-      <c r="B441" s="36"/>
-      <c r="C441" s="37" t="s">
+      <c r="A441" s="7"/>
+      <c r="B441" s="8"/>
+      <c r="C441" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="D441" s="38"/>
+      <c r="D441" s="3"/>
     </row>
     <row r="442" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A442" s="35"/>
-      <c r="B442" s="36"/>
-      <c r="C442" s="37" t="s">
+      <c r="A442" s="7"/>
+      <c r="B442" s="8"/>
+      <c r="C442" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="D442" s="38"/>
+      <c r="D442" s="3"/>
     </row>
     <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="35"/>
-      <c r="B443" s="36"/>
-      <c r="C443" s="37" t="s">
+      <c r="A443" s="7"/>
+      <c r="B443" s="8"/>
+      <c r="C443" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="D443" s="38"/>
+      <c r="D443" s="3"/>
     </row>
     <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A444" s="35"/>
-      <c r="B444" s="36"/>
-      <c r="C444" s="37" t="s">
+      <c r="A444" s="7"/>
+      <c r="B444" s="8"/>
+      <c r="C444" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="D444" s="38"/>
+      <c r="D444" s="3"/>
     </row>
     <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A445" s="35"/>
-      <c r="B445" s="36"/>
-      <c r="C445" s="37" t="s">
+      <c r="A445" s="7"/>
+      <c r="B445" s="8"/>
+      <c r="C445" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="D445" s="38"/>
+      <c r="D445" s="3"/>
     </row>
     <row r="446" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A446" s="35"/>
-      <c r="B446" s="36"/>
-      <c r="C446" s="37" t="s">
+      <c r="A446" s="7"/>
+      <c r="B446" s="8"/>
+      <c r="C446" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="D446" s="38"/>
+      <c r="D446" s="3"/>
     </row>
     <row r="447" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A447" s="35"/>
-      <c r="B447" s="36"/>
-      <c r="C447" s="37" t="s">
+      <c r="A447" s="7"/>
+      <c r="B447" s="8"/>
+      <c r="C447" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="D447" s="38"/>
+      <c r="D447" s="3"/>
     </row>
     <row r="448" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A448" s="35"/>
-      <c r="B448" s="36"/>
-      <c r="C448" s="39" t="s">
+      <c r="A448" s="7"/>
+      <c r="B448" s="8"/>
+      <c r="C448" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="D448" s="38"/>
+      <c r="D448" s="3"/>
     </row>
     <row r="449" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="35"/>
-      <c r="B449" s="36"/>
-      <c r="C449" s="37" t="s">
+      <c r="A449" s="7"/>
+      <c r="B449" s="8"/>
+      <c r="C449" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="D449" s="38"/>
+      <c r="D449" s="3"/>
     </row>
     <row r="450" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="35"/>
-      <c r="B450" s="36"/>
-      <c r="C450" s="37" t="s">
+      <c r="A450" s="7"/>
+      <c r="B450" s="8"/>
+      <c r="C450" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="D450" s="38"/>
+      <c r="D450" s="3"/>
     </row>
     <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A451" s="35"/>
-      <c r="B451" s="36"/>
-      <c r="C451" s="37" t="s">
+      <c r="A451" s="7"/>
+      <c r="B451" s="8"/>
+      <c r="C451" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="D451" s="38"/>
+      <c r="D451" s="3"/>
     </row>
     <row r="452" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A452" s="35"/>
-      <c r="B452" s="36"/>
-      <c r="C452" s="37" t="s">
+      <c r="A452" s="7"/>
+      <c r="B452" s="8"/>
+      <c r="C452" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="D452" s="38"/>
+      <c r="D452" s="3"/>
     </row>
     <row r="453" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A453" s="35"/>
-      <c r="B453" s="36"/>
-      <c r="C453" s="37" t="s">
+      <c r="A453" s="7"/>
+      <c r="B453" s="8"/>
+      <c r="C453" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="D453" s="38"/>
+      <c r="D453" s="3"/>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A454" s="46"/>
-      <c r="B454" s="43" t="s">
+      <c r="A454" s="9"/>
+      <c r="B454" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C454" s="43"/>
-      <c r="D454" s="43"/>
+      <c r="C454" s="27"/>
+      <c r="D454" s="27"/>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="9" t="s">
@@ -6321,544 +6281,544 @@
       <c r="D461" s="3"/>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A462" s="48"/>
-      <c r="B462" s="49" t="s">
+      <c r="A462" s="37"/>
+      <c r="B462" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C462" s="49"/>
-      <c r="D462" s="49"/>
+      <c r="C462" s="38"/>
+      <c r="D462" s="38"/>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A463" s="48"/>
-      <c r="B463" s="49"/>
-      <c r="C463" s="50"/>
-      <c r="D463" s="51"/>
+      <c r="A463" s="37"/>
+      <c r="B463" s="38"/>
+      <c r="C463" s="39"/>
+      <c r="D463" s="40"/>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A464" s="48"/>
-      <c r="B464" s="49"/>
-      <c r="C464" s="50"/>
-      <c r="D464" s="51"/>
+      <c r="A464" s="37"/>
+      <c r="B464" s="38"/>
+      <c r="C464" s="39"/>
+      <c r="D464" s="40"/>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A465" s="48"/>
-      <c r="B465" s="49"/>
-      <c r="C465" s="50"/>
-      <c r="D465" s="51"/>
+      <c r="A465" s="37"/>
+      <c r="B465" s="38"/>
+      <c r="C465" s="39"/>
+      <c r="D465" s="40"/>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A466" s="48"/>
-      <c r="B466" s="49"/>
-      <c r="C466" s="50"/>
-      <c r="D466" s="51"/>
+      <c r="A466" s="37"/>
+      <c r="B466" s="38"/>
+      <c r="C466" s="39"/>
+      <c r="D466" s="40"/>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A467" s="48"/>
-      <c r="B467" s="49"/>
-      <c r="C467" s="50"/>
-      <c r="D467" s="51"/>
+      <c r="A467" s="37"/>
+      <c r="B467" s="38"/>
+      <c r="C467" s="39"/>
+      <c r="D467" s="40"/>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A468" s="48"/>
-      <c r="B468" s="49"/>
-      <c r="C468" s="50"/>
-      <c r="D468" s="51"/>
+      <c r="A468" s="37"/>
+      <c r="B468" s="38"/>
+      <c r="C468" s="39"/>
+      <c r="D468" s="40"/>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A469" s="48"/>
-      <c r="B469" s="49"/>
-      <c r="C469" s="50"/>
-      <c r="D469" s="51"/>
+      <c r="A469" s="37"/>
+      <c r="B469" s="38"/>
+      <c r="C469" s="39"/>
+      <c r="D469" s="40"/>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A470" s="48"/>
-      <c r="B470" s="49"/>
-      <c r="C470" s="50"/>
-      <c r="D470" s="51"/>
+      <c r="A470" s="37"/>
+      <c r="B470" s="38"/>
+      <c r="C470" s="39"/>
+      <c r="D470" s="40"/>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A471" s="48"/>
-      <c r="B471" s="49"/>
-      <c r="C471" s="50"/>
-      <c r="D471" s="51"/>
+      <c r="A471" s="37"/>
+      <c r="B471" s="38"/>
+      <c r="C471" s="39"/>
+      <c r="D471" s="40"/>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A472" s="48"/>
-      <c r="B472" s="49"/>
-      <c r="C472" s="50"/>
-      <c r="D472" s="51"/>
+      <c r="A472" s="37"/>
+      <c r="B472" s="38"/>
+      <c r="C472" s="39"/>
+      <c r="D472" s="40"/>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A473" s="48"/>
-      <c r="B473" s="49"/>
-      <c r="C473" s="50"/>
-      <c r="D473" s="51"/>
+      <c r="A473" s="37"/>
+      <c r="B473" s="38"/>
+      <c r="C473" s="39"/>
+      <c r="D473" s="40"/>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A474" s="48"/>
-      <c r="B474" s="49"/>
-      <c r="C474" s="50"/>
-      <c r="D474" s="51"/>
+      <c r="A474" s="37"/>
+      <c r="B474" s="38"/>
+      <c r="C474" s="39"/>
+      <c r="D474" s="40"/>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="48"/>
-      <c r="B475" s="49"/>
-      <c r="C475" s="50"/>
-      <c r="D475" s="51"/>
+      <c r="A475" s="37"/>
+      <c r="B475" s="38"/>
+      <c r="C475" s="39"/>
+      <c r="D475" s="40"/>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A476" s="48"/>
-      <c r="B476" s="49"/>
-      <c r="C476" s="50"/>
-      <c r="D476" s="51"/>
+      <c r="A476" s="37"/>
+      <c r="B476" s="38"/>
+      <c r="C476" s="39"/>
+      <c r="D476" s="40"/>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A477" s="48"/>
-      <c r="B477" s="49"/>
-      <c r="C477" s="50"/>
-      <c r="D477" s="51"/>
+      <c r="A477" s="37"/>
+      <c r="B477" s="38"/>
+      <c r="C477" s="39"/>
+      <c r="D477" s="40"/>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A478" s="48"/>
-      <c r="B478" s="49"/>
-      <c r="C478" s="50"/>
-      <c r="D478" s="51"/>
+      <c r="A478" s="37"/>
+      <c r="B478" s="38"/>
+      <c r="C478" s="39"/>
+      <c r="D478" s="40"/>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A479" s="48"/>
-      <c r="B479" s="49"/>
-      <c r="C479" s="50"/>
-      <c r="D479" s="51"/>
+      <c r="A479" s="37"/>
+      <c r="B479" s="38"/>
+      <c r="C479" s="39"/>
+      <c r="D479" s="40"/>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A480" s="48"/>
-      <c r="B480" s="49"/>
-      <c r="C480" s="50"/>
-      <c r="D480" s="51"/>
+      <c r="A480" s="37"/>
+      <c r="B480" s="38"/>
+      <c r="C480" s="39"/>
+      <c r="D480" s="40"/>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A481" s="48"/>
-      <c r="B481" s="49"/>
-      <c r="C481" s="50"/>
-      <c r="D481" s="51"/>
+      <c r="A481" s="37"/>
+      <c r="B481" s="38"/>
+      <c r="C481" s="39"/>
+      <c r="D481" s="40"/>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="48"/>
-      <c r="B482" s="49"/>
-      <c r="C482" s="50"/>
-      <c r="D482" s="51"/>
+      <c r="A482" s="37"/>
+      <c r="B482" s="38"/>
+      <c r="C482" s="39"/>
+      <c r="D482" s="40"/>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A483" s="48"/>
-      <c r="B483" s="49"/>
-      <c r="C483" s="50"/>
-      <c r="D483" s="51"/>
+      <c r="A483" s="37"/>
+      <c r="B483" s="38"/>
+      <c r="C483" s="39"/>
+      <c r="D483" s="40"/>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A484" s="48"/>
-      <c r="B484" s="49"/>
-      <c r="C484" s="50"/>
-      <c r="D484" s="51"/>
+      <c r="A484" s="37"/>
+      <c r="B484" s="38"/>
+      <c r="C484" s="39"/>
+      <c r="D484" s="40"/>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="9"/>
       <c r="B485" s="9"/>
       <c r="C485" s="5"/>
-      <c r="D485" s="51"/>
+      <c r="D485" s="40"/>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C486" s="5"/>
-      <c r="D486" s="51"/>
+      <c r="D486" s="40"/>
     </row>
     <row r="487" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A487" s="52" t="s">
+      <c r="A487" s="41" t="s">
         <v>358</v>
       </c>
-      <c r="B487" s="52"/>
-      <c r="C487" s="53"/>
-      <c r="D487" s="54"/>
+      <c r="B487" s="41"/>
+      <c r="C487" s="42"/>
+      <c r="D487" s="43"/>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A488" s="55" t="s">
+      <c r="A488" s="44" t="s">
         <v>359</v>
       </c>
-      <c r="B488" s="56" t="s">
+      <c r="B488" s="45" t="s">
         <v>360</v>
       </c>
-      <c r="C488" s="57"/>
-      <c r="D488" s="56"/>
+      <c r="C488" s="46"/>
+      <c r="D488" s="45"/>
     </row>
     <row r="489" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A489" s="55" t="s">
+      <c r="A489" s="44" t="s">
         <v>361</v>
       </c>
-      <c r="B489" s="58" t="s">
+      <c r="B489" s="47" t="s">
         <v>362</v>
       </c>
-      <c r="C489" s="52"/>
-      <c r="D489" s="58"/>
+      <c r="C489" s="41"/>
+      <c r="D489" s="47"/>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A490" s="55" t="s">
+      <c r="A490" s="44" t="s">
         <v>363</v>
       </c>
-      <c r="B490" s="56" t="s">
+      <c r="B490" s="45" t="s">
         <v>364</v>
       </c>
-      <c r="C490" s="56"/>
-      <c r="D490" s="56"/>
+      <c r="C490" s="45"/>
+      <c r="D490" s="45"/>
     </row>
     <row r="491" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A491" s="55" t="s">
+      <c r="A491" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="B491" s="59" t="s">
+      <c r="B491" s="48" t="s">
         <v>366</v>
       </c>
-      <c r="C491" s="59"/>
-      <c r="D491" s="59"/>
+      <c r="C491" s="48"/>
+      <c r="D491" s="48"/>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A492" s="55" t="s">
+      <c r="A492" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="B492" s="60" t="s">
+      <c r="B492" s="49" t="s">
         <v>368</v>
       </c>
-      <c r="C492" s="60"/>
-      <c r="D492" s="60"/>
+      <c r="C492" s="49"/>
+      <c r="D492" s="49"/>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A493" s="55" t="s">
+      <c r="A493" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="B493" s="58" t="s">
+      <c r="B493" s="47" t="s">
         <v>370</v>
       </c>
-      <c r="C493" s="61"/>
-      <c r="D493" s="58"/>
+      <c r="C493" s="50"/>
+      <c r="D493" s="47"/>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A494" s="55" t="s">
+      <c r="A494" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="B494" s="58" t="s">
+      <c r="B494" s="47" t="s">
         <v>372</v>
       </c>
-      <c r="C494" s="58"/>
-      <c r="D494" s="58"/>
+      <c r="C494" s="47"/>
+      <c r="D494" s="47"/>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A495" s="55" t="s">
+      <c r="A495" s="44" t="s">
         <v>373</v>
       </c>
-      <c r="B495" s="56" t="s">
+      <c r="B495" s="45" t="s">
         <v>374</v>
       </c>
-      <c r="C495" s="58"/>
-      <c r="D495" s="56"/>
+      <c r="C495" s="47"/>
+      <c r="D495" s="45"/>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A496" s="53" t="s">
+      <c r="A496" s="42" t="s">
         <v>375</v>
       </c>
-      <c r="B496" s="58" t="s">
+      <c r="B496" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="C496" s="58"/>
-      <c r="D496" s="58"/>
+      <c r="C496" s="47"/>
+      <c r="D496" s="47"/>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A497" s="55" t="s">
+      <c r="A497" s="44" t="s">
         <v>377</v>
       </c>
-      <c r="B497" s="58" t="s">
+      <c r="B497" s="47" t="s">
         <v>360</v>
       </c>
-      <c r="C497" s="56"/>
-      <c r="D497" s="58"/>
+      <c r="C497" s="45"/>
+      <c r="D497" s="47"/>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A498" s="55" t="s">
+      <c r="A498" s="44" t="s">
         <v>378</v>
       </c>
-      <c r="B498" s="58" t="s">
+      <c r="B498" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="C498" s="58"/>
-      <c r="D498" s="58"/>
+      <c r="C498" s="47"/>
+      <c r="D498" s="47"/>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A499" s="62" t="s">
+      <c r="A499" s="51" t="s">
         <v>380</v>
       </c>
-      <c r="B499" s="63" t="s">
+      <c r="B499" s="52" t="s">
         <v>381</v>
       </c>
-      <c r="C499" s="64"/>
-      <c r="D499" s="63"/>
+      <c r="C499" s="53"/>
+      <c r="D499" s="52"/>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A500" s="55" t="s">
+      <c r="A500" s="44" t="s">
         <v>382</v>
       </c>
-      <c r="B500" s="58" t="s">
+      <c r="B500" s="47" t="s">
         <v>383</v>
       </c>
-      <c r="C500" s="58"/>
-      <c r="D500" s="58"/>
+      <c r="C500" s="47"/>
+      <c r="D500" s="47"/>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A501" s="65" t="s">
+      <c r="A501" s="54" t="s">
         <v>384</v>
       </c>
-      <c r="B501" s="58" t="s">
+      <c r="B501" s="47" t="s">
         <v>385</v>
       </c>
-      <c r="C501" s="58"/>
-      <c r="D501" s="58"/>
+      <c r="C501" s="47"/>
+      <c r="D501" s="47"/>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A502" s="65" t="s">
+      <c r="A502" s="54" t="s">
         <v>386</v>
       </c>
-      <c r="B502" s="58" t="s">
+      <c r="B502" s="47" t="s">
         <v>387</v>
       </c>
-      <c r="C502" s="58"/>
-      <c r="D502" s="58"/>
+      <c r="C502" s="47"/>
+      <c r="D502" s="47"/>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A503" s="66" t="s">
+      <c r="A503" s="55" t="s">
         <v>388</v>
       </c>
-      <c r="B503" s="67" t="s">
+      <c r="B503" s="56" t="s">
         <v>389</v>
       </c>
-      <c r="C503" s="67"/>
-      <c r="D503" s="67"/>
+      <c r="C503" s="56"/>
+      <c r="D503" s="56"/>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A504" s="66" t="s">
+      <c r="A504" s="55" t="s">
         <v>390</v>
       </c>
-      <c r="B504" s="68" t="s">
+      <c r="B504" s="57" t="s">
         <v>391</v>
       </c>
-      <c r="C504" s="68"/>
-      <c r="D504" s="68"/>
+      <c r="C504" s="57"/>
+      <c r="D504" s="57"/>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="66" t="s">
+      <c r="A505" s="55" t="s">
         <v>392</v>
       </c>
-      <c r="B505" s="67" t="s">
+      <c r="B505" s="56" t="s">
         <v>393</v>
       </c>
-      <c r="C505" s="67"/>
-      <c r="D505" s="67"/>
+      <c r="C505" s="56"/>
+      <c r="D505" s="56"/>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A506" s="69" t="s">
+      <c r="A506" s="58" t="s">
         <v>394</v>
       </c>
-      <c r="B506" s="70" t="s">
+      <c r="B506" s="59" t="s">
         <v>395</v>
       </c>
-      <c r="C506" s="70"/>
-      <c r="D506" s="70"/>
+      <c r="C506" s="59"/>
+      <c r="D506" s="59"/>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A507" s="66" t="s">
+      <c r="A507" s="55" t="s">
         <v>396</v>
       </c>
-      <c r="B507" s="68" t="s">
+      <c r="B507" s="57" t="s">
         <v>397</v>
       </c>
-      <c r="C507" s="68"/>
-      <c r="D507" s="68"/>
+      <c r="C507" s="57"/>
+      <c r="D507" s="57"/>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A508" s="66" t="s">
+      <c r="A508" s="55" t="s">
         <v>398</v>
       </c>
-      <c r="B508" s="68" t="s">
+      <c r="B508" s="57" t="s">
         <v>399</v>
       </c>
-      <c r="C508" s="68"/>
-      <c r="D508" s="68"/>
+      <c r="C508" s="57"/>
+      <c r="D508" s="57"/>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A509" s="71" t="s">
+      <c r="A509" s="60" t="s">
         <v>400</v>
       </c>
-      <c r="B509" s="72" t="s">
+      <c r="B509" s="61" t="s">
         <v>401</v>
       </c>
-      <c r="C509" s="72"/>
-      <c r="D509" s="72"/>
+      <c r="C509" s="61"/>
+      <c r="D509" s="61"/>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A510" s="71"/>
-      <c r="B510" s="72"/>
-      <c r="C510" s="72"/>
-      <c r="D510" s="72"/>
+      <c r="A510" s="60"/>
+      <c r="B510" s="61"/>
+      <c r="C510" s="61"/>
+      <c r="D510" s="61"/>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A511" s="66" t="s">
+      <c r="A511" s="55" t="s">
         <v>402</v>
       </c>
-      <c r="B511" s="68" t="s">
+      <c r="B511" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="C511" s="68"/>
-      <c r="D511" s="68"/>
+      <c r="C511" s="57"/>
+      <c r="D511" s="57"/>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A512" s="66" t="s">
+      <c r="A512" s="55" t="s">
         <v>404</v>
       </c>
-      <c r="B512" s="68" t="s">
+      <c r="B512" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="C512" s="68"/>
-      <c r="D512" s="68"/>
+      <c r="C512" s="57"/>
+      <c r="D512" s="57"/>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A513" s="67" t="s">
+      <c r="A513" s="56" t="s">
         <v>406</v>
       </c>
-      <c r="B513" s="73" t="s">
+      <c r="B513" s="62" t="s">
         <v>407</v>
       </c>
-      <c r="C513" s="73"/>
-      <c r="D513" s="73"/>
+      <c r="C513" s="62"/>
+      <c r="D513" s="62"/>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A514" s="67"/>
-      <c r="B514" s="73"/>
-      <c r="C514" s="73"/>
-      <c r="D514" s="73"/>
+      <c r="A514" s="56"/>
+      <c r="B514" s="62"/>
+      <c r="C514" s="62"/>
+      <c r="D514" s="62"/>
     </row>
     <row r="515" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="B515" s="74" t="s">
+      <c r="B515" s="63" t="s">
         <v>409</v>
       </c>
-      <c r="C515" s="74"/>
-      <c r="D515" s="74"/>
+      <c r="C515" s="63"/>
+      <c r="D515" s="63"/>
     </row>
     <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="0" t="s">
         <v>410</v>
       </c>
-      <c r="B516" s="74" t="s">
+      <c r="B516" s="63" t="s">
         <v>411</v>
       </c>
-      <c r="C516" s="74"/>
-      <c r="D516" s="74"/>
+      <c r="C516" s="63"/>
+      <c r="D516" s="63"/>
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="0" t="s">
         <v>412</v>
       </c>
-      <c r="B517" s="74" t="s">
+      <c r="B517" s="63" t="s">
         <v>413</v>
       </c>
-      <c r="C517" s="74"/>
-      <c r="D517" s="74"/>
+      <c r="C517" s="63"/>
+      <c r="D517" s="63"/>
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D518" s="75"/>
+      <c r="D518" s="64"/>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D519" s="76"/>
+      <c r="D519" s="65"/>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D520" s="76"/>
+      <c r="D520" s="65"/>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D521" s="76"/>
+      <c r="D521" s="65"/>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D522" s="76"/>
+      <c r="D522" s="65"/>
     </row>
     <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A523" s="77" t="s">
+      <c r="A523" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B523" s="78" t="s">
+      <c r="B523" s="67" t="s">
         <v>145</v>
       </c>
-      <c r="C523" s="79"/>
-      <c r="D523" s="76"/>
+      <c r="C523" s="68"/>
+      <c r="D523" s="65"/>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="9"/>
-      <c r="B524" s="80" t="s">
+      <c r="B524" s="69" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A525" s="81" t="s">
+      <c r="A525" s="70" t="s">
         <v>50</v>
       </c>
       <c r="B525" s="21" t="s">
         <v>414</v>
       </c>
-      <c r="C525" s="82"/>
+      <c r="C525" s="71"/>
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A526" s="81"/>
+      <c r="A526" s="70"/>
       <c r="B526" s="21"/>
-      <c r="C526" s="83"/>
+      <c r="C526" s="72"/>
     </row>
     <row r="527" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A527" s="81"/>
+      <c r="A527" s="70"/>
       <c r="B527" s="21"/>
       <c r="C527" s="4" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A528" s="81"/>
+      <c r="A528" s="70"/>
       <c r="B528" s="21"/>
       <c r="C528" s="4" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A529" s="81"/>
+      <c r="A529" s="70"/>
       <c r="B529" s="21"/>
       <c r="C529" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A530" s="81"/>
+      <c r="A530" s="70"/>
       <c r="B530" s="21"/>
       <c r="C530" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A531" s="81"/>
+      <c r="A531" s="70"/>
       <c r="B531" s="21"/>
       <c r="C531" s="4" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A532" s="81"/>
+      <c r="A532" s="70"/>
       <c r="B532" s="21"/>
       <c r="C532" s="4" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A533" s="81"/>
+      <c r="A533" s="70"/>
       <c r="B533" s="21"/>
       <c r="C533" s="4" t="s">
         <v>417</v>
@@ -6866,7 +6826,7 @@
     </row>
     <row r="534" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="9"/>
-      <c r="B534" s="84" t="s">
+      <c r="B534" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C534" s="4" t="s">
@@ -7534,9 +7494,8 @@
     <mergeCell ref="B525:B533"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B165" r:id="rId1" display="Prerequisite: Open link &quot;https://inventory.edu-netcracker.com/pages/startpage.xhtml&quot;"/>
-    <hyperlink ref="B456" r:id="rId2" display="Prerequisite: 1) Pre-registration in the system 2) Open link &quot;https://inventory.edu-netcracker.com/pages/inventory/inventory.xhtml?id=2&quot;"/>
-    <hyperlink ref="B516" r:id="rId3" display="Username — random username; Password - &quot;19032001stR+&quot;; Confirm password - same with Password; e-mail: «pink-b@listru»."/>
+    <hyperlink ref="B456" r:id="rId1" display="Prerequisite: 1) Pre-registration in the system 2) Open link &quot;https://inventory.edu-netcracker.com/pages/inventory/inventory.xhtml?id=2&quot;"/>
+    <hyperlink ref="B516" r:id="rId2" display="Username — random username; Password - &quot;19032001stR+&quot;; Confirm password - same with Password; e-mail: «pink-b@listru»."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7555,8 +7514,8 @@
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7571,7 +7530,7 @@
       <c r="A1" s="0" t="s">
         <v>420</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="74" t="s">
         <v>421</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -7582,12 +7541,12 @@
       <c r="A2" s="0" t="s">
         <v>422</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="75" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="75" t="s">
         <v>424</v>
       </c>
     </row>
@@ -7595,7 +7554,7 @@
       <c r="A4" s="0" t="s">
         <v>425</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="76" t="s">
         <v>426</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -7606,131 +7565,131 @@
       <c r="A5" s="0" t="s">
         <v>427</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="76" t="s">
         <v>428</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="77" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="78" t="s">
         <v>429</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="78" t="s">
         <v>430</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="77" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="77" t="s">
         <v>431</v>
       </c>
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="78" t="s">
         <v>432</v>
       </c>
-      <c r="C7" s="88" t="s">
+      <c r="C7" s="77" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="77" t="s">
         <v>433</v>
       </c>
-      <c r="B8" s="90" t="s">
+      <c r="B8" s="79" t="s">
         <v>434</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="77" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="77" t="s">
         <v>435</v>
       </c>
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="78" t="s">
         <v>436</v>
       </c>
-      <c r="C9" s="88" t="s">
+      <c r="C9" s="77" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="77" t="s">
         <v>437</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="80" t="s">
         <v>438</v>
       </c>
-      <c r="C10" s="88" t="s">
+      <c r="C10" s="77" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="88" t="s">
+      <c r="A11" s="77" t="s">
         <v>440</v>
       </c>
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="78" t="s">
         <v>441</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="77" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="77" t="s">
         <v>442</v>
       </c>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="78" t="s">
         <v>443</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="77" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="77" t="s">
         <v>444</v>
       </c>
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="78" t="s">
         <v>445</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="77" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="77" t="s">
         <v>446</v>
       </c>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="81" t="s">
         <v>447</v>
       </c>
-      <c r="C14" s="88" t="s">
+      <c r="C14" s="77" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="88" t="s">
+      <c r="A15" s="77" t="s">
         <v>449</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="81" t="s">
         <v>450</v>
       </c>
-      <c r="C15" s="88" t="s">
+      <c r="C15" s="77" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="77" t="s">
         <v>452</v>
       </c>
-      <c r="B16" s="89" t="s">
+      <c r="B16" s="78" t="s">
         <v>453</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C16" s="77" t="s">
         <v>171</v>
       </c>
     </row>
@@ -7749,86 +7708,86 @@
     <row r="19" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="88"/>
-      <c r="B21" s="93" t="s">
+      <c r="A21" s="77"/>
+      <c r="B21" s="82" t="s">
         <v>456</v>
       </c>
-      <c r="C21" s="88"/>
+      <c r="C21" s="77"/>
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="88" t="s">
+      <c r="A22" s="77" t="s">
         <v>457</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="76" t="s">
         <v>458</v>
       </c>
-      <c r="C22" s="88" t="s">
+      <c r="C22" s="77" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="88"/>
-      <c r="B23" s="93" t="s">
+      <c r="A23" s="77"/>
+      <c r="B23" s="82" t="s">
         <v>459</v>
       </c>
-      <c r="C23" s="88"/>
+      <c r="C23" s="77"/>
     </row>
     <row r="24" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="77" t="s">
         <v>460</v>
       </c>
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="76" t="s">
         <v>461</v>
       </c>
-      <c r="C24" s="88" t="s">
+      <c r="C24" s="77" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="88" t="s">
+      <c r="A25" s="77" t="s">
         <v>463</v>
       </c>
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="76" t="s">
         <v>464</v>
       </c>
-      <c r="C25" s="88" t="s">
+      <c r="C25" s="77" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="77" t="s">
         <v>466</v>
       </c>
-      <c r="B26" s="87" t="s">
+      <c r="B26" s="76" t="s">
         <v>467</v>
       </c>
-      <c r="C26" s="88" t="s">
+      <c r="C26" s="77" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="83" t="s">
         <v>469</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="84" t="s">
         <v>470</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="83" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="88"/>
-      <c r="B28" s="87"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="76"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="87"/>
+      <c r="B29" s="76"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>472</v>
       </c>
-      <c r="B30" s="93" t="s">
+      <c r="B30" s="82" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7836,7 +7795,7 @@
       <c r="A31" s="0" t="s">
         <v>474</v>
       </c>
-      <c r="B31" s="89" t="s">
+      <c r="B31" s="78" t="s">
         <v>475</v>
       </c>
     </row>
@@ -7844,7 +7803,7 @@
       <c r="A32" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="B32" s="89" t="s">
+      <c r="B32" s="78" t="s">
         <v>477</v>
       </c>
     </row>
@@ -7852,7 +7811,7 @@
       <c r="A33" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="B33" s="89" t="s">
+      <c r="B33" s="78" t="s">
         <v>479</v>
       </c>
     </row>
@@ -7860,7 +7819,7 @@
       <c r="A34" s="0" t="s">
         <v>480</v>
       </c>
-      <c r="B34" s="89" t="s">
+      <c r="B34" s="78" t="s">
         <v>481</v>
       </c>
     </row>

</xml_diff>